<commit_message>
2.3.3: Dynamic Clause: NOT IN and NOT BETWEEN are implemented.
</commit_message>
<xml_diff>
--- a/test/data/sqlite/SampleSQLite002.xlsx
+++ b/test/data/sqlite/SampleSQLite002.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/test/data/sqlite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B77DCA60-1D46-C44E-9562-DCA6D1D550CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{674A915E-F4A3-D045-BBE9-7A206802E7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="4120" windowWidth="22460" windowHeight="17540" tabRatio="457"/>
+    <workbookView xWindow="18220" yWindow="1420" windowWidth="22460" windowHeight="17540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sql" sheetId="38" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <definedName name="論理演算子">config!$J$5:$J$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -737,13 +738,7 @@
   <si>
     <t>簡易なSQLのサンプルです。</t>
     <rPh sb="0" eb="2">
-      <t xml:space="preserve">カンイナ </t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t xml:space="preserve">ジョウホウ </t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t xml:space="preserve">ナクナル </t>
+      <t xml:space="preserve">カンイナ ジョウホウ ナクナル </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1150,31 +1145,7 @@
       <t xml:space="preserve">ソクチ </t>
     </rPh>
     <rPh sb="5" eb="6">
-      <t xml:space="preserve">アタエル </t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t xml:space="preserve">オナジ </t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t xml:space="preserve">タイシテ </t>
-    </rPh>
-    <rPh sb="19" eb="22">
-      <t xml:space="preserve">ジョウケンクタイプ </t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t xml:space="preserve">タイショウ </t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t xml:space="preserve">アタイノ </t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t xml:space="preserve">カタ </t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t xml:space="preserve">イッチ </t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t xml:space="preserve">ヒツヨウガ </t>
+      <t xml:space="preserve">アタエル オナジ タイシテ ジョウケンクタイプ タイショウ アタイノ カタ イッチ ヒツヨウガ </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1182,7 +1153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2027,14 +1998,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3501,34 +3472,34 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>期待する処理件数</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>SQLタイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:C39 C18:C24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:C39 C18:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>パラメータタイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>スクロール属性空白付</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>更新可能属性</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>動的SQL</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>入力パラメータBean</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D34" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>条件句タイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F34" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>比較演算子</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28:G34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28:G34" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>繰り返し時演算子</formula1>
     </dataValidation>
   </dataValidations>
@@ -3539,14 +3510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
2.3.4: ITEMONLY type is deprecated. ORDERBY type is now available.
</commit_message>
<xml_diff>
--- a/test/data/sqlite/SampleSQLite002.xlsx
+++ b/test/data/sqlite/SampleSQLite002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/test/data/sqlite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{674A915E-F4A3-D045-BBE9-7A206802E7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{24092F4B-2C84-B543-A876-35F888AD174F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18220" yWindow="1420" windowWidth="22460" windowHeight="17540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="152">
   <si>
     <t>パラメータ名</t>
     <rPh sb="5" eb="6">
@@ -710,13 +710,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ITEMONLY</t>
-  </si>
-  <si>
-    <t>ITEMONLY</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>AND</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -837,10 +830,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>order by ${ORDERBY}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>-- ITEMONLY は複数カラム指定するとカンマ区切りで出力することとする</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1148,6 +1137,13 @@
       <t xml:space="preserve">アタエル オナジ タイシテ ジョウケンクタイプ タイショウ アタイノ カタ イッチ ヒツヨウガ </t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${ORDERBY}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ORDERBY</t>
   </si>
 </sst>
 </file>
@@ -2004,8 +2000,8 @@
   </sheetPr>
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2086,7 +2082,7 @@
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="15" t="s">
@@ -2104,7 +2100,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="15" t="s">
@@ -2122,7 +2118,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -2275,18 +2271,18 @@
         <v>74</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="53" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H18" s="54"/>
       <c r="I18" s="54"/>
@@ -2298,13 +2294,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
@@ -2414,16 +2410,16 @@
         <v>79</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H27" s="70" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I27" s="21" t="s">
         <v>80</v>
@@ -2435,26 +2431,26 @@
         <v>74</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H28" s="27" t="s">
         <v>30</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J28" s="68"/>
     </row>
@@ -2464,26 +2460,26 @@
         <v>2</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D29" s="27" t="s">
         <v>81</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H29" s="27" t="s">
         <v>28</v>
       </c>
       <c r="I29" s="69" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J29" s="68"/>
     </row>
@@ -2493,31 +2489,31 @@
         <v>3</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F30" s="27" t="s">
         <v>85</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H30" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J30" s="68" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2526,28 +2522,28 @@
         <v>4</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>83</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H31" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J31" s="68"/>
     </row>
@@ -2557,22 +2553,22 @@
         <v>5</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="I32" s="69" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J32" s="68"/>
     </row>
@@ -2667,7 +2663,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="37" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
@@ -2681,7 +2677,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -2695,7 +2691,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -2764,12 +2760,12 @@
     </row>
     <row r="50" spans="1:13" ht="13.5" customHeight="1">
       <c r="A50" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
       <c r="D50" s="74" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38"/>
@@ -2783,7 +2779,7 @@
     </row>
     <row r="51" spans="1:13" ht="13.5" customHeight="1">
       <c r="A51" s="66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -2800,12 +2796,12 @@
     </row>
     <row r="52" spans="1:13" ht="13.5" customHeight="1">
       <c r="A52" s="66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="43"/>
       <c r="D52" s="73" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
@@ -2819,12 +2815,12 @@
     </row>
     <row r="53" spans="1:13" ht="13.5" customHeight="1">
       <c r="A53" s="66" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
       <c r="D53" s="73" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="73"/>
@@ -2838,12 +2834,12 @@
     </row>
     <row r="54" spans="1:13" ht="13.5" customHeight="1">
       <c r="A54" s="66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
       <c r="D54" s="73" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E54" s="43"/>
       <c r="F54" s="73"/>
@@ -2857,7 +2853,7 @@
     </row>
     <row r="55" spans="1:13" ht="13.5" customHeight="1">
       <c r="A55" s="66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
@@ -2874,7 +2870,7 @@
     </row>
     <row r="56" spans="1:13" ht="13.5" customHeight="1">
       <c r="A56" s="66" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
@@ -2891,12 +2887,12 @@
     </row>
     <row r="57" spans="1:13" ht="13.5" customHeight="1">
       <c r="A57" s="66" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
@@ -2910,12 +2906,12 @@
     </row>
     <row r="58" spans="1:13" ht="13.5" customHeight="1">
       <c r="A58" s="66" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
       <c r="D58" s="73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
@@ -3517,7 +3513,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3576,7 +3572,7 @@
         <v>93</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3608,7 +3604,7 @@
         <v>86</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3640,7 +3636,7 @@
         <v>89</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3658,7 +3654,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>90</v>
@@ -3674,7 +3670,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>87</v>
@@ -3689,7 +3685,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I9" s="72" t="s">
         <v>88</v>
@@ -3704,7 +3700,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>91</v>
@@ -3720,7 +3716,7 @@
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:10">

</xml_diff>

<commit_message>
2.3.5: bug fix. comparisons are defined as just EQ, and missing NE.
</commit_message>
<xml_diff>
--- a/test/data/sqlite/SampleSQLite002.xlsx
+++ b/test/data/sqlite/SampleSQLite002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/test/data/sqlite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{24092F4B-2C84-B543-A876-35F888AD174F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{D9A325AB-8D4F-3B48-87CD-F95245DDF9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18220" yWindow="1420" windowWidth="22460" windowHeight="17540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <definedName name="条件句タイプ">config!$H$5:$H$11</definedName>
     <definedName name="動的SQL">config!$F$5:$F$7</definedName>
     <definedName name="入力パラメータBean">config!$G$5:$G$7</definedName>
-    <definedName name="比較演算子">config!$I$5:$I$12</definedName>
+    <definedName name="比較演算子">config!$I$5:$I$13</definedName>
     <definedName name="論理演算子">config!$J$5:$J$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
   <si>
     <t>パラメータ名</t>
     <rPh sb="5" eb="6">
@@ -667,9 +667,6 @@
   </si>
   <si>
     <t>EQ</t>
-  </si>
-  <si>
-    <t>EQ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1144,6 +1141,13 @@
   </si>
   <si>
     <t>ORDERBY</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NE</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -2001,7 +2005,7 @@
   <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2082,7 +2086,7 @@
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="15" t="s">
@@ -2100,7 +2104,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="15" t="s">
@@ -2118,7 +2122,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -2271,18 +2275,18 @@
         <v>74</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="53" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18" s="54"/>
       <c r="I18" s="54"/>
@@ -2294,13 +2298,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
@@ -2410,16 +2414,16 @@
         <v>79</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G27" s="70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H27" s="70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I27" s="21" t="s">
         <v>80</v>
@@ -2431,26 +2435,26 @@
         <v>74</v>
       </c>
       <c r="B28" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>117</v>
-      </c>
       <c r="D28" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H28" s="27" t="s">
         <v>30</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J28" s="68"/>
     </row>
@@ -2460,26 +2464,26 @@
         <v>2</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" s="27" t="s">
         <v>81</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="27" t="s">
         <v>28</v>
       </c>
       <c r="I29" s="69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J29" s="68"/>
     </row>
@@ -2489,31 +2493,31 @@
         <v>3</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H30" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J30" s="68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2522,28 +2526,28 @@
         <v>4</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>83</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H31" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J31" s="68"/>
     </row>
@@ -2553,22 +2557,22 @@
         <v>5</v>
       </c>
       <c r="B32" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>127</v>
-      </c>
       <c r="D32" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="I32" s="69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J32" s="68"/>
     </row>
@@ -2663,7 +2667,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
@@ -2677,7 +2681,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -2691,7 +2695,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -2760,12 +2764,12 @@
     </row>
     <row r="50" spans="1:13" ht="13.5" customHeight="1">
       <c r="A50" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
       <c r="D50" s="74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38"/>
@@ -2779,7 +2783,7 @@
     </row>
     <row r="51" spans="1:13" ht="13.5" customHeight="1">
       <c r="A51" s="66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -2796,12 +2800,12 @@
     </row>
     <row r="52" spans="1:13" ht="13.5" customHeight="1">
       <c r="A52" s="66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="43"/>
       <c r="D52" s="73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
@@ -2815,12 +2819,12 @@
     </row>
     <row r="53" spans="1:13" ht="13.5" customHeight="1">
       <c r="A53" s="66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
       <c r="D53" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="73"/>
@@ -2834,12 +2838,12 @@
     </row>
     <row r="54" spans="1:13" ht="13.5" customHeight="1">
       <c r="A54" s="66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
       <c r="D54" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E54" s="43"/>
       <c r="F54" s="73"/>
@@ -2853,7 +2857,7 @@
     </row>
     <row r="55" spans="1:13" ht="13.5" customHeight="1">
       <c r="A55" s="66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
@@ -2870,7 +2874,7 @@
     </row>
     <row r="56" spans="1:13" ht="13.5" customHeight="1">
       <c r="A56" s="66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
@@ -2887,12 +2891,12 @@
     </row>
     <row r="57" spans="1:13" ht="13.5" customHeight="1">
       <c r="A57" s="66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
@@ -2906,12 +2910,12 @@
     </row>
     <row r="58" spans="1:13" ht="13.5" customHeight="1">
       <c r="A58" s="66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
       <c r="D58" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
@@ -3513,7 +3517,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3569,10 +3573,10 @@
         <v>79</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3601,10 +3605,10 @@
         <v>84</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3633,10 +3637,10 @@
         <v>82</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3654,10 +3658,10 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J7" s="13"/>
     </row>
@@ -3670,10 +3674,10 @@
         <v>22</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>87</v>
+        <v>110</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3685,10 +3689,10 @@
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" s="72" t="s">
-        <v>88</v>
+        <v>112</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3700,10 +3704,10 @@
         <v>24</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>91</v>
+        <v>125</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3716,7 +3720,7 @@
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="8" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3727,7 +3731,9 @@
       <c r="E12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="8" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="7"/>
@@ -3737,6 +3743,7 @@
       <c r="E13" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:10">
       <c r="E14" s="11" t="s">

</xml_diff>